<commit_message>
edited and 3. case added
</commit_message>
<xml_diff>
--- a/data/invalidLogin.xlsx
+++ b/data/invalidLogin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre\Desktop\tobeto_Platform\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F456AD-D93D-4610-A13F-A05A4F3E4706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A2ECD5-6ADD-4EBD-A00B-9E6148195ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,16 +39,16 @@
     <t>basarisiztest</t>
   </si>
   <si>
-    <t>basarisiz3@test.com</t>
-  </si>
-  <si>
-    <t>basarisiz2@test.com</t>
-  </si>
-  <si>
     <t>basarisiztest3</t>
   </si>
   <si>
     <t>testbasarisiz</t>
+  </si>
+  <si>
+    <t>test@basarisiz.com</t>
+  </si>
+  <si>
+    <t>basarisiz@basarisiz.com</t>
   </si>
 </sst>
 </file>
@@ -380,12 +380,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -407,18 +407,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>